<commit_message>
Add Python code to create redirects and also move source files
Signed-off-by: tpmccallum <tim.mccallum@fermyon.com>
</commit_message>
<xml_diff>
--- a/migration_scripts/mapping_information.xlsx
+++ b/migration_scripts/mapping_information.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C83"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,752 +429,1254 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>file_path</t>
+          <t>original_file_path</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>toc_label</t>
+          <t>unified_file_path</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>original_toc_label</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>unified_toc_label</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/"</t>
+          <t>/spin/v2/</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Introduction</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/quickstart"</t>
+          <t>/spin/v2/quickstart</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Quickstart</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/install"</t>
+          <t>/spin/v2/install</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Install</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/upgrade"</t>
+          <t>/spin/v2/upgrade</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Upgrade</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/see-what-people-have-built-with-spin"</t>
+          <t>/spin/v2/see-what-people-have-built-with-spin</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Built With Spin</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/writing-apps"</t>
+          <t>/spin/v2/writing-apps</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Writing Applications</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/spin-application-structure"</t>
+          <t>/spin/v2/spin-application-structure</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Structuring Applications</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/build"</t>
+          <t>/spin/v2/build</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Compiling Applications</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/testing-apps"</t>
+          <t>/spin/v2/testing-apps</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Testing Applications</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/running-apps"</t>
+          <t>/spin/v2/running-apps</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Running Applications</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/distributing-apps"</t>
+          <t>/spin/v2/distributing-apps</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Publishing and Distribution</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/observing-apps"</t>
+          <t>/spin/v2/observing-apps</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Observing Applications</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/troubleshooting-application-dev"</t>
+          <t>/spin/v2/troubleshooting-application-dev</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Troubleshooting Application Development</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/language-support-overview"</t>
+          <t>/spin/v2/language-support-overview</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Language Support Overview</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/rust-components"</t>
+          <t>/spin/v2/rust-components</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Rust</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/go-components"</t>
+          <t>/spin/v2/go-components</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Go</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/javascript-components"</t>
+          <t>/spin/v2/javascript-components</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Javascript</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/python-components"</t>
+          <t>/spin/v2/python-components</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/other-languages"</t>
+          <t>/spin/v2/other-languages</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Other Languages</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/triggers"</t>
+          <t>/spin/v2/triggers</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Triggers</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/http-trigger"</t>
+          <t>/spin/v2/http-trigger</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>The HTTP Trigger</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/redis-trigger"</t>
+          <t>/spin/v2/redis-trigger</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>The Redis Trigger</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/api-guides-overview"</t>
+          <t>/spin/v2/api-guides-overview</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>API Support Overview</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/http-outbound"</t>
+          <t>/spin/v2/http-outbound</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Making HTTP Requests</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/kv-store-api-guide"</t>
+          <t>/spin/v2/kv-store-api-guide</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Key Value Store</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/mqtt-outbound"</t>
+          <t>/spin/v2/mqtt-outbound</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>MQTT Messaging</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/serverless-ai-api-guide"</t>
+          <t>/spin/v2/serverless-ai-api-guide</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Serverless AI</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/sqlite-api-guide"</t>
+          <t>/spin/v2/sqlite-api-guide</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>SQLite Storage</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/redis-outbound"</t>
+          <t>/spin/v2/redis-outbound</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Redis Storage</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/rdbms-storage"</t>
+          <t>/spin/v2/rdbms-storage</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Relational Database Storage</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/variables"</t>
+          <t>/spin/v2/variables</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Application Variables</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/serverless-ai-hello-world.md"</t>
+          <t>/spin/v2/serverless-ai-hello-world.md</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Build Your First Serverless AI App</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/ai-sentiment-analysis-api-tutorial"</t>
+          <t>/spin/v2/ai-sentiment-analysis-api-tutorial</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Sentiment Analysis With Serverless AI</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/url-shortener-tutorial"</t>
+          <t>/spin/v2/url-shortener-tutorial</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Building a URL Shortener With Spin</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/registry-tutorial"</t>
+          <t>/spin/v2/registry-tutorial</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Spin Apps in Registries</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/key-value-store-tutorial"</t>
+          <t>/spin/v2/key-value-store-tutorial</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Spin Key-Value Store</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/managing-templates"</t>
+          <t>/spin/v2/managing-templates</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Managing Templates</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/managing-plugins"</t>
+          <t>/spin/v2/managing-plugins</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Managing Plugins</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/cli-reference"</t>
+          <t>/spin/v2/cli-reference</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>CLI Reference</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/manifest-reference-v1"</t>
+          <t>/spin/v2/manifest-reference-v1</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Application Manifest (Version 1) Reference</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/manifest-reference"</t>
+          <t>/spin/v2/manifest-reference</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Application Manifest Reference</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/wasm-languages/webassembly-language-support"</t>
+          <t>/wasm-languages/webassembly-language-support</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>WebAssembly Language Support Matrix</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/extending-and-embedding"</t>
+          <t>/spin/v2/extending-and-embedding</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Extending and Embedding Spin</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/deploying-to-fermyon"</t>
+          <t>/spin/v2/deploying-to-fermyon</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
       <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Deploying to Fermyon</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/architecture/"</t>
+          <t>/spin/v2/architecture/</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Architecture</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/dynamic-configuration"</t>
+          <t>/spin/v2/dynamic-configuration</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Dynamic Application Configuration</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/cache"</t>
+          <t>/spin/v2/cache</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Spin Internal Data Layout</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/template-authoring"</t>
+          <t>/spin/v2/template-authoring</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Creating Spin Templates</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/plugin-authoring"</t>
+          <t>/spin/v2/plugin-authoring</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Creating Spin Plugins</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/kubernetes"</t>
+          <t>/spin/v2/kubernetes</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Spin on Kubernetes</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/spin-in-pods-legacy"</t>
+          <t>/spin/v2/spin-in-pods-legacy</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
       <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Spin in Pods (Legacy)</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/contributing-docs"</t>
+          <t>/spin/v2/contributing-docs</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
       <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Contributing to Docs</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/spin/v2/contributing-spin"</t>
+          <t>/spin/v2/contributing-spin</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Contributing to Spin</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/"</t>
+          <t>/cloud/</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Introduction</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/quickstart"</t>
+          <t>/cloud/quickstart</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr"/>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Quickstart</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/develop"</t>
+          <t>/cloud/develop</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Develop a Spin Application</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/deploy"</t>
+          <t>/cloud/deploy</t>
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
       <c r="C58" t="inlineStr"/>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Deploy an Application</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/upgrade"</t>
+          <t>/cloud/upgrade</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Upgrade an Application</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/delete"</t>
+          <t>/cloud/delete</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
       <c r="C60" t="inlineStr"/>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Delete an Application</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/fermyon-cloud"</t>
+          <t>/cloud/fermyon-cloud</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr"/>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>The Fermyon Cloud</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/deployment-concepts"</t>
+          <t>/cloud/deployment-concepts</t>
         </is>
       </c>
       <c r="B62" t="inlineStr"/>
       <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Deployment Concepts</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/custom-domain"</t>
+          <t>/cloud/custom-domain</t>
         </is>
       </c>
       <c r="B63" t="inlineStr"/>
       <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Custom Domain</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/linking-applications-to-resources-using-labels"</t>
+          <t>/cloud/linking-applications-to-resources-using-labels</t>
         </is>
       </c>
       <c r="B64" t="inlineStr"/>
       <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Linking Apps To Resources Using Labels</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/spin-vs-code-extension"</t>
+          <t>/cloud/spin-vs-code-extension</t>
         </is>
       </c>
       <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Using VS Code Extension</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/kv-cloud-tutorial"</t>
+          <t>/cloud/kv-cloud-tutorial</t>
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
       <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Cloud Key-Value Store</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/noops-sql-db"</t>
+          <t>/cloud/noops-sql-db</t>
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Persisting Data With SQLite Database</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/data-redis"</t>
+          <t>/cloud/data-redis</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Persisting Data With Redis</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/data-postgres"</t>
+          <t>/cloud/data-postgres</t>
         </is>
       </c>
       <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Persisting Data With PostgreSQL</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/github-actions"</t>
+          <t>/cloud/github-actions</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
       <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Deploying Spin Apps Using GitHub Action</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/custom-fermyon-subdomain"</t>
+          <t>/cloud/custom-fermyon-subdomain</t>
         </is>
       </c>
       <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Apply Custom Fermyon Subdomain</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/custom-domains-tutorial"</t>
+          <t>/cloud/custom-domains-tutorial</t>
         </is>
       </c>
       <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr"/>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Apply Custom Domain</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/variables"</t>
+          <t>/cloud/variables</t>
         </is>
       </c>
       <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr"/>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Configuring App Variables and Secrets</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/rest-api"</t>
+          <t>/cloud/rest-api</t>
         </is>
       </c>
       <c r="B74" t="inlineStr"/>
       <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>REST API</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/cli-reference"</t>
+          <t>/cloud/cli-reference</t>
         </is>
       </c>
       <c r="B75" t="inlineStr"/>
       <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Spin CLI Reference</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/cloud-command-reference"</t>
+          <t>/cloud/cloud-command-reference</t>
         </is>
       </c>
       <c r="B76" t="inlineStr"/>
       <c r="C76" t="inlineStr"/>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Cloud Command Reference</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/changelog"</t>
+          <t>/cloud/changelog</t>
         </is>
       </c>
       <c r="B77" t="inlineStr"/>
       <c r="C77" t="inlineStr"/>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Changelog</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/wasm-languages/webassembly-language-support"</t>
+          <t>/wasm-languages/webassembly-language-support</t>
         </is>
       </c>
       <c r="B78" t="inlineStr"/>
       <c r="C78" t="inlineStr"/>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>WebAssembly Language Support Matrix</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/user-settings"</t>
+          <t>/cloud/user-settings</t>
         </is>
       </c>
       <c r="B79" t="inlineStr"/>
       <c r="C79" t="inlineStr"/>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>The User Settings Screen</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/faq"</t>
+          <t>/cloud/faq</t>
         </is>
       </c>
       <c r="B80" t="inlineStr"/>
       <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Quotas, Limitations, and Technical FAQ</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/pricing-and-billing"</t>
+          <t>/cloud/pricing-and-billing</t>
         </is>
       </c>
       <c r="B81" t="inlineStr"/>
       <c r="C81" t="inlineStr"/>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Pricing and Billing</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/support"</t>
+          <t>/cloud/support</t>
         </is>
       </c>
       <c r="B82" t="inlineStr"/>
       <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>How to Get Help?</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>href="{{site.info.base_url}}/cloud/contributing-docs"</t>
+          <t>/cloud/contributing-docs</t>
         </is>
       </c>
       <c r="B83" t="inlineStr"/>
       <c r="C83" t="inlineStr"/>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Contributing to Docs</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>